<commit_message>
testing yml link file
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="4995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,6 +603,30 @@
         <f>F3</f>
         <v>04/01/2022</v>
       </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H9" si="0">"---
+date: " &amp; F4 &amp; "
+layout: entry
+name: " &amp; A4 &amp; "
+description: " &amp; B4 &amp; " 
+link: " &amp; C4 &amp; "
+categories:
+" &amp; E4 &amp; "
+tags:
+" &amp; D4 &amp; "
+---"</f>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: Cloudflared addon for HA
+description: … 
+link: https://github.com/brenner-tobias/addon-cloudflared
+categories:
+ - HA
+tags:
+ - HA
+---</v>
+      </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
@@ -628,6 +652,20 @@
         <f>F4</f>
         <v>04/01/2022</v>
       </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: More on Cloudflared
+description: … 
+link: https://community.home-assistant.io/t/new-add-on-cloudflared/361637
+categories:
+ - HA
+tags:
+ - HA
+---</v>
+      </c>
       <c r="J5" t="s">
         <v>14</v>
       </c>
@@ -653,6 +691,20 @@
         <f>F5</f>
         <v>04/01/2022</v>
       </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: reddit on Cloudflared
+description: … 
+link: https://www.reddit.com/r/homeassistant/comments/sh1u3y/anybody_using_the_cloudflared_addon_for_remote/
+categories:
+ - HA
+tags:
+ - HA
+---</v>
+      </c>
       <c r="J6" t="s">
         <v>14</v>
       </c>
@@ -678,6 +730,20 @@
         <f>F6</f>
         <v>04/01/2022</v>
       </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: getting started with home assistant core installing
+description: mainly for starting HA at boot 
+link: https://www.raspberryfield.life/2020/06/14/getting-started-with-home-assistant-core-installing/
+categories:
+ - HA
+tags:
+ - HA
+---</v>
+      </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
@@ -703,6 +769,20 @@
         <f>F7</f>
         <v>04/01/2022</v>
       </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: How to add Sunrise &amp; Sunset Cards
+description: … 
+link: https://community.home-assistant.io/t/how-to-add-sunrise-sunset-cards/109545
+categories:
+ - HA
+tags:
+ - HA
+---</v>
+      </c>
       <c r="J8" t="s">
         <v>14</v>
       </c>
@@ -727,6 +807,20 @@
       <c r="F9" s="3" t="str">
         <f>F8</f>
         <v>04/01/2022</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>---
+date: 04/01/2022
+layout: entry
+name: Setting the value of a helper from the weather temperature attribute
+description: to create a sensor with external hourly temperature 
+link: https://community.home-assistant.io/t/setting-the-value-of-a-helper-from-the-weather-temperature-attribute/371230/4
+categories:
+ - HA
+tags:
+ - HA
+---</v>
       </c>
       <c r="J9" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
moving to links db for all posts and links page
</commit_message>
<xml_diff>
--- a/links.xlsx
+++ b/links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="91">
   <si>
     <t>https://requestmetrics.com/web-performance/http3-is-fast</t>
   </si>
@@ -60,9 +60,6 @@
     <t>date</t>
   </si>
   <si>
-    <t xml:space="preserve"> - web</t>
-  </si>
-  <si>
     <t>04/01/2022</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>Cloudflared addon for HA</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - HA</t>
-  </si>
-  <si>
     <t>https://community.home-assistant.io/t/new-add-on-cloudflared/361637</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>links:</t>
   </si>
   <si>
-    <t>web</t>
-  </si>
-  <si>
     <t>HA</t>
   </si>
   <si>
@@ -147,14 +135,176 @@
     <t>https://www.youtube.com/watch?v=A5SaixJE3mI</t>
   </si>
   <si>
-    <t>security</t>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Jekyll</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Jekyll, Web</t>
+  </si>
+  <si>
+    <t>Web, Security</t>
+  </si>
+  <si>
+    <t>for loop sorted collection</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/Phlow/1f27dfafdf2bbcc5c48e</t>
+  </si>
+  <si>
+    <t>This loop loops through a collection called `collection_name`</t>
+  </si>
+  <si>
+    <t>https://github.com/kalkih/mini-graph-card</t>
+  </si>
+  <si>
+    <t>Lovelace Mini Graph Card</t>
+  </si>
+  <si>
+    <t>https://thenextweb.com/news/good-microsoft-store-apps</t>
+  </si>
+  <si>
+    <t>Our favorite free Windows 11 apps from the Microsoft Store</t>
+  </si>
+  <si>
+    <t>especially for "Journal"</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>using Jekyll as a DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to move to a links table instead of individual pages </t>
+  </si>
+  <si>
+    <t>https://github.com/rypan/jekyll-db</t>
+  </si>
+  <si>
+    <t>14/02/2022</t>
+  </si>
+  <si>
+    <t>Generate and Decode QR Codes using Python</t>
+  </si>
+  <si>
+    <t>https://python.plainenglish.io/all-notes-to-generate-and-decode-qr-codes-using-python-a745072db7fe</t>
+  </si>
+  <si>
+    <t>Adam Marczak - Microsoft Azure Fundamentals</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLGjZwEtPN7j-Q59JYso3L4_yoCjj2syrM</t>
+  </si>
+  <si>
+    <t>Studying</t>
+  </si>
+  <si>
+    <t>home assistand backup to Google Drive</t>
+  </si>
+  <si>
+    <t>https://github.com/sabeechen/hassio-google-drive-backup</t>
+  </si>
+  <si>
+    <t>reddit post on SD vs SSD drives for HA</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/homeassistant/comments/ltvdnp/sd_versus_usb_flash_drive_versus_ssd_for_home/</t>
+  </si>
+  <si>
+    <t>Introduction to Flask AppBuilder — Build a Simple Web Service</t>
+  </si>
+  <si>
+    <t>https://python.plainenglish.io/introduction-to-flask-appbuilder-building-a-simple-web-service-16ad26876ef6</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>31/01/2022</t>
+  </si>
+  <si>
+    <t>https://twitter.com/edent/status/1484131697461547016</t>
+  </si>
+  <si>
+    <t>twitter - migrating away from g-suite</t>
+  </si>
+  <si>
+    <t>potential write up on migrating away from g-suite</t>
+  </si>
+  <si>
+    <t>https://community.home-assistant.io/t/7-day-accumulated-rain-fall/14984/6</t>
+  </si>
+  <si>
+    <t>7 Day accumulated rain fall</t>
+  </si>
+  <si>
+    <t>to help figure out if i run off road or not</t>
+  </si>
+  <si>
+    <t>24/01/2022</t>
+  </si>
+  <si>
+    <t>https://github.com/EBOOZ/TeamsStatus</t>
+  </si>
+  <si>
+    <t>Teams Status in Home Assistant</t>
+  </si>
+  <si>
+    <t>but not to use for Teams, just a general strategy for pushing data to HA</t>
+  </si>
+  <si>
+    <t>17/01/2021</t>
+  </si>
+  <si>
+    <t>https://www.tsia.com/blog/what-is-the-fish-model</t>
+  </si>
+  <si>
+    <t>What Is the Fish Model?</t>
+  </si>
+  <si>
+    <t>10/02/2021</t>
+  </si>
+  <si>
+    <t>EASY Lovelace Mobile Dashboard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5y6rhwr5Y8c</t>
+  </si>
+  <si>
+    <t>04/01/2021</t>
+  </si>
+  <si>
+    <t>https://www.tablesgenerator.com/markdown_tables</t>
+  </si>
+  <si>
+    <t>Markdown Table Generator</t>
+  </si>
+  <si>
+    <t>Massively Theme on Jekyll home</t>
+  </si>
+  <si>
+    <t>https://iwiedenm.github.io/jekyll-theme-massively/</t>
+  </si>
+  <si>
+    <t>Markdown Reference</t>
+  </si>
+  <si>
+    <t>https://www.markdownguide.org/extended-syntax/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +316,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,12 +356,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -489,11 +649,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -504,29 +666,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>30</v>
+      <c r="H1" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -540,24 +702,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="str">
-        <f>IF(A2&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A2&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B2&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C2&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F2&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E2,"")</f>
+        <f>IF(A2&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A2&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B2&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C2&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F2&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E2&amp;$G$1&amp;"   "&amp;$D$1&amp;": "&amp;D2,"")</f>
         <v xml:space="preserve"> - name: HTTP/3 is Fast
    description:  via https://danielmiessler.com/
    link: https://requestmetrics.com/web-performance/http3-is-fast
    date: 04/01/2022
-   tags: web</v>
+   category: Web
+   tags: Web</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -568,233 +731,225 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H40" si="0">IF(A3&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A3&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B3&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C3&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F3&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E3,"")</f>
+        <f t="shared" ref="H3:H10" si="0">IF(A3&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A3&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B3&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C3&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F3&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E3&amp;$G$1&amp;"   "&amp;$D$1&amp;": "&amp;D3,"")</f>
         <v xml:space="preserve"> - name: QUIC vs TCP+TLS — and why QUIC is not the next big thing
    description: 
    link: https://medium.com/codavel-blog/quic-vs-tcp-tls-and-why-quic-is-not-the-next-big-thing-d4ef59143efd
    date: 04/01/2022
-   tags: web</v>
+   category: Web
+   tags: Web</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="str">
-        <f t="shared" ref="F4:F9" si="1">F3</f>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44227</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: Cloudflared addon for HA
-   description: …
+   description: 
    link: https://github.com/brenner-tobias/addon-cloudflared
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44227</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: More on Cloudflared
-   description: …
+   description: 
    link: https://community.home-assistant.io/t/new-add-on-cloudflared/361637
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F6" s="2">
+        <v>44227</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: reddit on Cloudflared
-   description: …
+   description: 
    link: https://www.reddit.com/r/homeassistant/comments/sh1u3y/anybody_using_the_cloudflared_addon_for_remote/
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44227</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: getting started with home assistant core installing
    description: mainly for starting HA at boot
    link: https://www.raspberryfield.life/2020/06/14/getting-started-with-home-assistant-core-installing/
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F8" s="2">
+        <v>44227</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: How to add Sunrise &amp; Sunset Cards
-   description: …
+   description: 
    link: https://community.home-assistant.io/t/how-to-add-sunrise-sunset-cards/109545
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>04/01/2022</v>
+        <v>28</v>
+      </c>
+      <c r="F9" s="2">
+        <v>44227</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> - name: Setting the value of a helper from the weather temperature attribute
    description: to create a sensor with external hourly temperature
    link: https://community.home-assistant.io/t/setting-the-value-of-a-helper-from-the-weather-temperature-attribute/371230/4
-   date: 04/01/2022
+   date: 44227
+   category: HA
    tags: HA</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -802,359 +957,771 @@
    description: for a better way to serve a links table
    link: https://medium.com/blueeast/jekyll-and-data-files-with-real-time-example-6ea704213111
    date: 21/02/2022
-   tags: web</v>
+   category: Jekyll
+   tags: Jekyll, Web</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A11&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A11&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B11&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C11&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F11&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E11&amp;$G$1&amp;"   "&amp;$D$1&amp;": "&amp;D11,"")</f>
         <v xml:space="preserve"> - name: JWTs And Why They Suck
    description:  by @roddux/Rory M -- Security BSides London
    link: https://www.youtube.com/watch?v=A5SaixJE3mI
    date: 21/02/2022
-   tags: security</v>
+   category: Security
+   tags: Web, Security</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" ref="H12:H52" si="1">IF(A12&lt;&gt;""," - "&amp;$A$1&amp;": "&amp;A12&amp;$G$1&amp;"   "&amp;$B$1&amp;": "&amp;B12&amp;$G$1&amp;"   "&amp;$C$1&amp;": "&amp;C12&amp;$G$1&amp;"   "&amp;$F$1&amp;": "&amp;F12&amp;$G$1&amp;"   "&amp;$E$1&amp;": "&amp;E12&amp;$G$1&amp;"   "&amp;$D$1&amp;": "&amp;D12,"")</f>
+        <v xml:space="preserve"> - name: for loop sorted collection
+   description: This loop loops through a collection called `collection_name`
+   link: https://gist.github.com/Phlow/1f27dfafdf2bbcc5c48e
+   date: 21/02/2022
+   category: Jekyll
+   tags: Jekyll, Web</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Lovelace Mini Graph Card
+   description: 
+   link: https://github.com/kalkih/mini-graph-card
+   date: 21/02/2022
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Our favorite free Windows 11 apps from the Microsoft Store
+   description: especially for "Journal"
+   link: https://thenextweb.com/news/good-microsoft-store-apps
+   date: 21/02/2022
+   category: General
+   tags: General</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: using Jekyll as a DB
+   description: to move to a links table instead of individual pages 
+   link: https://github.com/rypan/jekyll-db
+   date: 14/02/2022
+   category: Jekyll
+   tags: Jekyll, Web</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Generate and Decode QR Codes using Python
+   description: 
+   link: https://python.plainenglish.io/all-notes-to-generate-and-decode-qr-codes-using-python-a745072db7fe
+   date: 14/02/2022
+   category: General
+   tags: General</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Adam Marczak - Microsoft Azure Fundamentals
+   description: 
+   link: https://www.youtube.com/playlist?list=PLGjZwEtPN7j-Q59JYso3L4_yoCjj2syrM
+   date: 14/02/2022
+   category: Studying
+   tags: Studying</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: home assistand backup to Google Drive
+   description: 
+   link: https://github.com/sabeechen/hassio-google-drive-backup
+   date: 14/02/2022
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: reddit post on SD vs SSD drives for HA
+   description: 
+   link: https://www.reddit.com/r/homeassistant/comments/ltvdnp/sd_versus_usb_flash_drive_versus_ssd_for_home/
+   date: 14/02/2022
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Introduction to Flask AppBuilder — Build a Simple Web Service
+   description: 
+   link: https://python.plainenglish.io/introduction-to-flask-appbuilder-building-a-simple-web-service-16ad26876ef6
+   date: 31/01/2022
+   category: Python
+   tags: Python</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: twitter - migrating away from g-suite
+   description: potential write up on migrating away from g-suite
+   link: https://twitter.com/edent/status/1484131697461547016
+   date: 24/01/2022
+   category: General
+   tags: General</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: 7 Day accumulated rain fall
+   description: to help figure out if i run off road or not
+   link: https://community.home-assistant.io/t/7-day-accumulated-rain-fall/14984/6
+   date: 24/01/2022
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Teams Status in Home Assistant
+   description: but not to use for Teams, just a general strategy for pushing data to HA
+   link: https://github.com/EBOOZ/TeamsStatus
+   date: 17/01/2021
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: What Is the Fish Model?
+   description: 
+   link: https://www.tsia.com/blog/what-is-the-fish-model
+   date: 10/02/2021
+   category: General
+   tags: General</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: EASY Lovelace Mobile Dashboard
+   description: 
+   link: https://www.youtube.com/watch?v=5y6rhwr5Y8c
+   date: 04/01/2021
+   category: HA
+   tags: HA</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Markdown Table Generator
+   description: 
+   link: https://www.tablesgenerator.com/markdown_tables
+   date: 04/01/2021
+   category: General
+   tags: General</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Massively Theme on Jekyll home
+   description: 
+   link: https://iwiedenm.github.io/jekyll-theme-massively/
+   date: 04/01/2021
+   category: Jekyll
+   tags: Jekyll, Web</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - name: Markdown Reference
+   description: 
+   link: https://www.markdownguide.org/extended-syntax/
+   date: 04/01/2021
+   category: General
+   tags: General</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I51" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="I52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1165,5 +1732,6 @@
     <hyperlink ref="C10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>